<commit_message>
Started recursive column dataType checker.
</commit_message>
<xml_diff>
--- a/raw/TestExcel.xlsx
+++ b/raw/TestExcel.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshuablackhurst/source/repos/personal/excel/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2CE694C-E0B9-6C46-9D18-9392C3E97D19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3A93D6A-15DC-4645-8222-944F0F646F46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{48F68C04-5AB0-694C-9038-17EC4AFDE95E}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="36">
   <si>
     <t>Flight Id</t>
   </si>
@@ -155,6 +155,12 @@
   <si>
     <t>N39DJ</t>
   </si>
+  <si>
+    <t>3837h8</t>
+  </si>
+  <si>
+    <t>CJ 4</t>
+  </si>
 </sst>
 </file>
 
@@ -164,7 +170,7 @@
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -205,6 +211,12 @@
     <font>
       <sz val="9"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -661,10 +673,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BAA49AE-E38F-9841-AD79-7B45D8EF7BE0}">
-  <dimension ref="A1:L1268"/>
+  <dimension ref="A1:L1269"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -747,149 +759,159 @@
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" s="5">
+      <c r="A3" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="5">
+        <v>1307808</v>
+      </c>
+      <c r="C3" s="6">
+        <v>45384</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J3" s="5">
+        <v>26255</v>
+      </c>
+      <c r="K3" s="7">
+        <v>2.0700000000000003</v>
+      </c>
+      <c r="L3" s="8">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" s="5">
         <v>810442</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B4" s="5">
         <v>1274962</v>
-      </c>
-      <c r="C3" s="6">
-        <v>45383</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="J3" s="5">
-        <v>26107</v>
-      </c>
-      <c r="K3" s="7">
-        <v>3.1500000000000004</v>
-      </c>
-      <c r="L3" s="8">
-        <f>IF(AND(F3&lt;&gt;"Flexjet, LLC",H3="Light Jet"),K3*'[1]Pricing Logic'!$F$4,IF(AND(F3&lt;&gt;"Flexjet, LLC",H3="Midsize Jet"),K3*'[1]Pricing Logic'!$F$5,IF(AND(F3&lt;&gt;"Flexjet, LLC",H3="Super Mid Jet"),K3*'[1]Pricing Logic'!$F$6,IF(AND(F3&lt;&gt;"Flexjet, LLC",H3="Large Cabin"),K3*'[1]Pricing Logic'!$F$7,IF(AND(F3&lt;&gt;"Flexjet, LLC",H3="Helicopter"),K3*'[1]Pricing Logic'!$F$8,IF(AND(F3="Flexjet, LLC",H3="Light Jet"),K3*'[1]Pricing Logic'!$F$12,IF(AND(F3="Flexjet, LLC",H3="Midsize Jet"),K3*'[1]Pricing Logic'!$F$13,IF(AND(F3="Flexjet, LLC",H3="Super Mid Jet"),K3*'[1]Pricing Logic'!$F$14,IF(AND(F3="Flexjet, LLC",H3="Large Cabin"),K3*'[1]Pricing Logic'!$F$15,IF(AND(F3="Flexjet, LLC",H3="Airliner"),K3*'[1]Pricing Logic'!$F$16,""))))))))))</f>
-        <v>107.88750000000002</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" s="5">
-        <v>846738</v>
-      </c>
-      <c r="B4" s="5">
-        <v>1305608</v>
       </c>
       <c r="C4" s="6">
         <v>45383</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="J4" s="5">
-        <v>25713</v>
+        <v>26107</v>
       </c>
       <c r="K4" s="7">
-        <v>2.72</v>
+        <v>3.1500000000000004</v>
       </c>
       <c r="L4" s="8">
         <f>IF(AND(F4&lt;&gt;"Flexjet, LLC",H4="Light Jet"),K4*'[1]Pricing Logic'!$F$4,IF(AND(F4&lt;&gt;"Flexjet, LLC",H4="Midsize Jet"),K4*'[1]Pricing Logic'!$F$5,IF(AND(F4&lt;&gt;"Flexjet, LLC",H4="Super Mid Jet"),K4*'[1]Pricing Logic'!$F$6,IF(AND(F4&lt;&gt;"Flexjet, LLC",H4="Large Cabin"),K4*'[1]Pricing Logic'!$F$7,IF(AND(F4&lt;&gt;"Flexjet, LLC",H4="Helicopter"),K4*'[1]Pricing Logic'!$F$8,IF(AND(F4="Flexjet, LLC",H4="Light Jet"),K4*'[1]Pricing Logic'!$F$12,IF(AND(F4="Flexjet, LLC",H4="Midsize Jet"),K4*'[1]Pricing Logic'!$F$13,IF(AND(F4="Flexjet, LLC",H4="Super Mid Jet"),K4*'[1]Pricing Logic'!$F$14,IF(AND(F4="Flexjet, LLC",H4="Large Cabin"),K4*'[1]Pricing Logic'!$F$15,IF(AND(F4="Flexjet, LLC",H4="Airliner"),K4*'[1]Pricing Logic'!$F$16,""))))))))))</f>
-        <v>68.680000000000007</v>
+        <v>107.88750000000002</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="5">
-        <v>848449</v>
+        <v>846738</v>
       </c>
       <c r="B5" s="5">
-        <v>1307807</v>
+        <v>1305608</v>
       </c>
       <c r="C5" s="6">
         <v>45383</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>16</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="J5" s="5">
-        <v>26255</v>
+        <v>25713</v>
       </c>
       <c r="K5" s="7">
-        <v>2.0700000000000003</v>
+        <v>2.72</v>
       </c>
       <c r="L5" s="8">
         <f>IF(AND(F5&lt;&gt;"Flexjet, LLC",H5="Light Jet"),K5*'[1]Pricing Logic'!$F$4,IF(AND(F5&lt;&gt;"Flexjet, LLC",H5="Midsize Jet"),K5*'[1]Pricing Logic'!$F$5,IF(AND(F5&lt;&gt;"Flexjet, LLC",H5="Super Mid Jet"),K5*'[1]Pricing Logic'!$F$6,IF(AND(F5&lt;&gt;"Flexjet, LLC",H5="Large Cabin"),K5*'[1]Pricing Logic'!$F$7,IF(AND(F5&lt;&gt;"Flexjet, LLC",H5="Helicopter"),K5*'[1]Pricing Logic'!$F$8,IF(AND(F5="Flexjet, LLC",H5="Light Jet"),K5*'[1]Pricing Logic'!$F$12,IF(AND(F5="Flexjet, LLC",H5="Midsize Jet"),K5*'[1]Pricing Logic'!$F$13,IF(AND(F5="Flexjet, LLC",H5="Super Mid Jet"),K5*'[1]Pricing Logic'!$F$14,IF(AND(F5="Flexjet, LLC",H5="Large Cabin"),K5*'[1]Pricing Logic'!$F$15,IF(AND(F5="Flexjet, LLC",H5="Airliner"),K5*'[1]Pricing Logic'!$F$16,""))))))))))</f>
+        <v>68.680000000000007</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" s="5">
+        <v>848449</v>
+      </c>
+      <c r="B6" s="5">
+        <v>1307807</v>
+      </c>
+      <c r="C6" s="6">
+        <v>45383</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J6" s="5">
+        <v>26255</v>
+      </c>
+      <c r="K6" s="7">
+        <v>2.0700000000000003</v>
+      </c>
+      <c r="L6" s="8">
+        <f>IF(AND(F6&lt;&gt;"Flexjet, LLC",H6="Light Jet"),K6*'[1]Pricing Logic'!$F$4,IF(AND(F6&lt;&gt;"Flexjet, LLC",H6="Midsize Jet"),K6*'[1]Pricing Logic'!$F$5,IF(AND(F6&lt;&gt;"Flexjet, LLC",H6="Super Mid Jet"),K6*'[1]Pricing Logic'!$F$6,IF(AND(F6&lt;&gt;"Flexjet, LLC",H6="Large Cabin"),K6*'[1]Pricing Logic'!$F$7,IF(AND(F6&lt;&gt;"Flexjet, LLC",H6="Helicopter"),K6*'[1]Pricing Logic'!$F$8,IF(AND(F6="Flexjet, LLC",H6="Light Jet"),K6*'[1]Pricing Logic'!$F$12,IF(AND(F6="Flexjet, LLC",H6="Midsize Jet"),K6*'[1]Pricing Logic'!$F$13,IF(AND(F6="Flexjet, LLC",H6="Super Mid Jet"),K6*'[1]Pricing Logic'!$F$14,IF(AND(F6="Flexjet, LLC",H6="Large Cabin"),K6*'[1]Pricing Logic'!$F$15,IF(AND(F6="Flexjet, LLC",H6="Airliner"),K6*'[1]Pricing Logic'!$F$16,""))))))))))</f>
         <v>52.267500000000005</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="8"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="8"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="5"/>
@@ -18545,7 +18567,22 @@
       <c r="K1268" s="7"/>
       <c r="L1268" s="8"/>
     </row>
+    <row r="1269" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1269" s="5"/>
+      <c r="B1269" s="5"/>
+      <c r="C1269" s="6"/>
+      <c r="D1269" s="5"/>
+      <c r="E1269" s="5"/>
+      <c r="F1269" s="5"/>
+      <c r="G1269" s="5"/>
+      <c r="H1269" s="5"/>
+      <c r="I1269" s="5"/>
+      <c r="J1269" s="5"/>
+      <c r="K1269" s="7"/>
+      <c r="L1269" s="8"/>
+    </row>
   </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>